<commit_message>
Changes for Screenshot and reports
</commit_message>
<xml_diff>
--- a/LinkAiwaysFCFramework/TestData/FCdata.xlsx
+++ b/LinkAiwaysFCFramework/TestData/FCdata.xlsx
@@ -4,113 +4,229 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Adult" sheetId="1" r:id="rId1"/>
     <sheet name="Payment" sheetId="2" r:id="rId2"/>
     <sheet name="Routes" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+  <si>
+    <t>Pax 1</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Pradeep</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>ZXCV</t>
+  </si>
+  <si>
+    <t>MobileNo</t>
+  </si>
+  <si>
+    <t>EMail</t>
+  </si>
+  <si>
+    <t>lingeswar@goquo.com</t>
+  </si>
+  <si>
+    <t>Confirmmail</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>2000-BARANGAROO,NSW</t>
+  </si>
+  <si>
+    <t>Pax 2</t>
+  </si>
+  <si>
+    <t>Mstr.</t>
+  </si>
+  <si>
+    <t>Lingeswar</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>dob date</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>DOB Month</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>DOB Year</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2000-DARLING HARBOUR,NSW</t>
+  </si>
+  <si>
+    <t>Pax 3</t>
+  </si>
+  <si>
+    <t>ASDFD</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>3000-MELBOURNE,VIC</t>
+  </si>
+  <si>
+    <t>Paymentcardname</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Cardno</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>BillingName</t>
+  </si>
+  <si>
+    <t>billinglastname</t>
+  </si>
+  <si>
+    <t>GQ</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>25 SaiBaba</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Coimbatore</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Trip</t>
+  </si>
+  <si>
+    <t>One Way</t>
+  </si>
+  <si>
+    <t>Departurecity</t>
+  </si>
+  <si>
+    <t>BNE</t>
+  </si>
+  <si>
+    <t>ArrivalCity</t>
+  </si>
+  <si>
+    <t>OAG</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>July 2024</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>RYear</t>
+  </si>
+  <si>
+    <t>RDate</t>
+  </si>
   <si>
     <t>Adult</t>
   </si>
   <si>
-    <t>Firstname</t>
-  </si>
-  <si>
-    <t>Tamil</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>MobileNo</t>
-  </si>
-  <si>
-    <t>EMail</t>
-  </si>
-  <si>
-    <t>lingeswar@goquo.com</t>
-  </si>
-  <si>
-    <t>Confirmmail</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>2000-BARANGAROO,NSW</t>
-  </si>
-  <si>
-    <t>Paymentcardname</t>
-  </si>
-  <si>
-    <t>Cardno</t>
-  </si>
-  <si>
-    <t>4111111111111111</t>
-  </si>
-  <si>
-    <t>CVV</t>
-  </si>
-  <si>
-    <t>BillingName</t>
-  </si>
-  <si>
-    <t>billinglastname</t>
-  </si>
-  <si>
-    <t>GQ</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>25 SaiBaba</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>Coimbatore</t>
-  </si>
-  <si>
-    <t>Postcode</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>Departurecity</t>
-  </si>
-  <si>
-    <t>BNE</t>
-  </si>
-  <si>
-    <t>ArrivalCity</t>
-  </si>
-  <si>
-    <t>OAG</t>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Inf</t>
+  </si>
+  <si>
+    <t>cabinclass</t>
+  </si>
+  <si>
+    <t>pro select_out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -571,16 +687,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1047,30 +1163,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16.5714285714286" style="2" customWidth="1"/>
     <col min="2" max="2" width="25.7142857142857" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1086,16 +1201,16 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
-        <v>9876543210</v>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9876543210</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1103,21 +1218,151 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="lingeswar@goquo.com"/>
     <hyperlink ref="B6" r:id="rId1" display="lingeswar@goquo.com"/>
+    <hyperlink ref="B7" r:id="rId1" display="lingeswar@goquo.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1141,23 +1386,23 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1">
         <v>123</v>
@@ -1165,39 +1410,39 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1">
         <v>641001</v>
@@ -1205,7 +1450,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1">
         <v>9876543210</v>
@@ -1220,31 +1465,130 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:B3"/>
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="14.1428571428571" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.8571428571429" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.14285714285714" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="14.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="9.57142857142857"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1">
+        <v>13131232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>